<commit_message>
feat(CWL): `SafeValueBonus` patch for `ElementContainer`
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/EN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/EN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76139639-0AD4-40E8-BA3E-C4934D04D688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3084F67C-004D-4C19-A3CD-465159002410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8670" yWindow="1335" windowWidth="37590" windowHeight="19095" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="6105" windowWidth="25395" windowHeight="13290" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -474,21 +474,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>failed to create {0} id: {1}, type: {2}, it may be missing from current game
-CWL caught the exception and kept the game going
-if this is causing issues,  please check for outdated mods or disable {3} in the config file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;Missing {0}:{1}:{2}:{3}&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This class is missing or modified from your current game. 
-CWL kept the game going by replacing it with a safety cone.
-You should report the relevant information to mod author or CWL.
-Using this element(if usable) will let CWL purge it from your save.
-You may also keep the safety cone, CWL will restore it when the responsible mod functions again.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -768,11 +754,6 @@
     <t>cwl_warn_quest_id_thing</t>
   </si>
   <si>
-    <t>quest {0} is trying to use invalid id: "{1}"
-CWL kept the game going by replacing it with "{2}"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cwl_warn_quest_id_thing2</t>
   </si>
   <si>
@@ -1019,12 +1000,6 @@
   <si>
     <t>cwl_warn_drama_play_ex</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Error occurred during drama play!
-CWL caught the exception and kept the game going
-Please check the Player.log and mods.
-{0}</t>
   </si>
   <si>
     <t>auto gained element: {0}/{1} on {2}</t>
@@ -1283,11 +1258,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>removed invalid actCombat ID: {0} from {1}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>removed invalid listAbility ID: {0} from {1}</t>
+    <t>Error occurred during drama play!
+Please check the Player.log and mods.
+{0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quest {0} is trying to use invalid id: "{1}"
+CWL replaced it with "{2}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CWL removed invalid actCombat ID: {0} from {1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CWL removed invalid listAbility ID: {0} from {1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This class is missing or modified from your current game. 
+You should report the relevant information to mod author or CWL.
+Using this element(if usable) will let CWL purge it from your save.
+You may also keep the safety cone, CWL will restore it when the responsible mod functions again.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>failed to create {0} id: {1}, type: {2}, it may be missing from current game
+if this is causing issues,  please check for outdated mods or disable {3} in the config file</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1754,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1831,10 +1829,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
@@ -2298,16 +2296,16 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="116.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="93" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B46"/>
       <c r="C46" s="6" t="s">
-        <v>110</v>
+        <v>266</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>110</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2327,21 +2325,21 @@
         <v>108</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="209.25" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="186" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>112</v>
+        <v>265</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>112</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
@@ -2370,14 +2368,14 @@
     </row>
     <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
@@ -2404,13 +2402,13 @@
     </row>
     <row r="55" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="69.75" x14ac:dyDescent="0.2">
@@ -2440,10 +2438,10 @@
         <v>91</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.2">
@@ -2470,731 +2468,731 @@
     </row>
     <row r="61" spans="1:4" ht="46.5" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="69.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="46.5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="10" customFormat="1" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="10" customFormat="1" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="46.5" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="3" t="s">
-        <v>161</v>
+        <v>262</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>161</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="46.5" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="46.5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="13" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D101" s="14" t="s">
         <v>205</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="93" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="69.75" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="3" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B114" s="15"/>
       <c r="C114" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D114" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="48.75" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B116" s="15"/>
       <c r="C116" s="17" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D116" s="16" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" s="15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B117" s="15"/>
       <c r="C117" s="18" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B118" s="15"/>
       <c r="C118" s="18" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D118" s="15" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A119" s="15" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B119" s="15"/>
       <c r="C119" s="19" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B120" s="15"/>
       <c r="C120" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D120" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B121" s="15"/>
       <c r="C121" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D121" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat(CWL): use script state and script cache
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/EN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/EN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95E32C7-4650-4C58-97BF-87017CFC4481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5796D8D8-4C97-4E96-A159-F3C1160B90CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1230" yWindow="735" windowWidth="30045" windowHeight="16095" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1661,9 +1661,6 @@
     <t>cwl_log_csc_roslyn</t>
   </si>
   <si>
-    <t>using roslyn compiler {0}</t>
-  </si>
-  <si>
     <t>cwl_log_csc_package</t>
   </si>
   <si>
@@ -1702,9 +1699,6 @@
     <t>script state '{0}' is frozen</t>
   </si>
   <si>
-    <t>Roslyn コンパイラを使用しています {0}</t>
-  </si>
-  <si>
     <t>{1} からパッケージ {0} をコンパイルしています</t>
   </si>
   <si>
@@ -1734,6 +1728,12 @@
   <si>
     <t>call failure: '{0}'
 {1}</t>
+  </si>
+  <si>
+    <t>using ℛ* compiler {0}</t>
+  </si>
+  <si>
+    <t>ℛ* コンパイラを使用しています {0}</t>
   </si>
 </sst>
 </file>
@@ -2258,10 +2258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -3793,10 +3793,10 @@
       </c>
       <c r="B129" s="15"/>
       <c r="C129" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D129" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="23.25">
@@ -3841,94 +3841,94 @@
       </c>
       <c r="B133" s="15"/>
       <c r="C133" s="15" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="D133" s="15" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="23.25">
       <c r="A134" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B134" s="15"/>
       <c r="C134" s="15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D134" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="46.5">
       <c r="A135" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B135" s="15"/>
       <c r="C135" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D135" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="23.25">
       <c r="A136" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B136" s="15"/>
       <c r="C136" s="15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D136" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="23.25">
       <c r="A137" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B137" s="15"/>
       <c r="C137" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D137" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="46.5">
       <c r="A138" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B138" s="15"/>
       <c r="C138" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D138" s="16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="23.25">
       <c r="A139" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B139" s="15"/>
       <c r="C139" s="15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D139" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="46.5">
       <c r="A140" s="26" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B140" s="15"/>
       <c r="C140" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D140" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="23.25">
@@ -3972,12 +3972,6 @@
       <c r="B147" s="15"/>
       <c r="C147" s="15"/>
       <c r="D147" s="15"/>
-    </row>
-    <row r="148" spans="1:4" ht="23.25">
-      <c r="A148" s="15"/>
-      <c r="B148" s="15"/>
-      <c r="C148" s="15"/>
-      <c r="D148" s="15"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D35">

</xml_diff>